<commit_message>
fixed all steps & improved account managment
</commit_message>
<xml_diff>
--- a/static/items.xlsx
+++ b/static/items.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Максим\Desktop\файлы для тестов Алексей\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Максим\Desktop\файлы скрипта с сервера\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDB6BE1-D6C7-4C84-91B6-B9196FC614C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E218F7-5A4D-4745-8FF1-11F2E708E99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="3450" windowWidth="18825" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8445" yWindow="2070" windowWidth="16635" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -39,22 +39,13 @@
     <t>Sleep</t>
   </si>
   <si>
-    <t>def; 0.15-0.18</t>
-  </si>
-  <si>
-    <t>SSG 08 | Abyss (Field-Tested)</t>
-  </si>
-  <si>
-    <t>0-23;0-23.58</t>
-  </si>
-  <si>
-    <t>Glock-18 | High Beam (Factory New)</t>
-  </si>
-  <si>
-    <t>def;0-0.01</t>
-  </si>
-  <si>
-    <t>0-17.49;0-17.58</t>
+    <t>Souvenir SSG 08 | Jungle Dashed (Battle-Scarred)</t>
+  </si>
+  <si>
+    <t>def;0.45-0.46</t>
+  </si>
+  <si>
+    <t>0-0.8;0-0.1</t>
   </si>
 </sst>
 </file>
@@ -381,17 +372,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" customWidth="1"/>
-    <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="1" max="1" width="47.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -410,31 +402,20 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
@@ -567,18 +548,6 @@
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>